<commit_message>
Modified the methods of reading binary files
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -11,11 +11,11 @@
     <sheet name="objdump" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="radare2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="angr" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="BAP" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Hopper" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="IDAPro" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Ghidra" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Dyninst" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="bap" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="hopper" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="idapro" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="ghidra" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="dyninst" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Statistics" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -482,7 +482,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -512,6 +512,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -587,7 +591,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1943,7 +1947,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BAP!$F$2:$F$52</c:f>
+              <c:f>bap!$F$2:$F$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2320,7 +2324,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hopper!$F$2:$F$52</c:f>
+              <c:f>hopper!$F$2:$F$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2697,7 +2701,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>IDAPro!$F$2:$F$52</c:f>
+              <c:f>idapro!$F$2:$F$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3074,7 +3078,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ghidra!$F$2:$F$52</c:f>
+              <c:f>ghidra!$F$2:$F$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3451,7 +3455,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dyninst!$F$2:$F$52</c:f>
+              <c:f>dyninst!$F$2:$F$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -3621,11 +3625,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="10860707"/>
-        <c:axId val="69122833"/>
+        <c:axId val="41104986"/>
+        <c:axId val="83761064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10860707"/>
+        <c:axId val="41104986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3653,7 +3657,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69122833"/>
+        <c:crossAx val="83761064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3661,7 +3665,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69122833"/>
+        <c:axId val="83761064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3698,7 +3702,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10860707"/>
+        <c:crossAx val="41104986"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3746,7 +3750,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9228,11 +9232,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="46190544"/>
-        <c:axId val="25284796"/>
+        <c:axId val="5684359"/>
+        <c:axId val="57265530"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46190544"/>
+        <c:axId val="5684359"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9260,7 +9264,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25284796"/>
+        <c:crossAx val="57265530"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9268,7 +9272,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="25284796"/>
+        <c:axId val="57265530"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -9298,7 +9302,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46190544"/>
+        <c:crossAx val="5684359"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9357,9 +9361,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>359640</xdr:colOff>
+      <xdr:colOff>358920</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>101880</xdr:rowOff>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9367,8 +9371,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8008920" y="175320"/>
-        <a:ext cx="10427760" cy="4152960"/>
+        <a:off x="8025840" y="175320"/>
+        <a:ext cx="10451880" cy="4152240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9380,16 +9384,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>585360</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>316800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>200160</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>138960</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>63720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9397,8 +9401,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7980480" y="5177160"/>
-        <a:ext cx="9474840" cy="4426560"/>
+        <a:off x="3611160" y="5389560"/>
+        <a:ext cx="9705240" cy="4427640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9422,7 +9426,7 @@
       <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -12022,7 +12026,7 @@
       <selection pane="topLeft" activeCell="I99" activeCellId="0" sqref="I99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -14642,7 +14646,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -17242,7 +17246,7 @@
       <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -20056,7 +20060,7 @@
       <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -24893,7 +24897,7 @@
       <selection pane="topLeft" activeCell="I99" activeCellId="0" sqref="I99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="11.54"/>
   </cols>
@@ -27522,7 +27526,7 @@
       <selection pane="topLeft" activeCell="C57" activeCellId="0" sqref="C57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -30320,13 +30324,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I104" activeCellId="0" sqref="I104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D35" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O62" activeCellId="0" sqref="O62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -33314,6 +33318,9 @@
       <c r="I103" s="5" t="n">
         <v>0.99044</v>
       </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I104" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>